<commit_message>
completed name and pathogen cleaning
</commit_message>
<xml_diff>
--- a/DataCleaning/mod_patients.xlsx
+++ b/DataCleaning/mod_patients.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="385">
   <si>
     <t>PatientName</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Marti F Perone</t>
   </si>
   <si>
-    <t>M Atkins;Tanaka, M E</t>
+    <t>Tanaka, M E;Atkins, M</t>
   </si>
   <si>
     <t>Aplysia kurodai;Sphenodon punctatus</t>
@@ -59,7 +59,7 @@
     <t>Merralee Ives Mcfarland</t>
   </si>
   <si>
-    <t>Mallorie A Barrowman;Mcallister, Rochelle C;Katerina Melack</t>
+    <t>Mcallister, Rochelle C;Barrowman, Mallorie A;Melack, Katerina</t>
   </si>
   <si>
     <t>Trinycteris nicefori</t>
@@ -71,7 +71,7 @@
     <t>Narayan, Rosalie</t>
   </si>
   <si>
-    <t>Blinnie Stimson;Mcallister, R C;R Mcallister</t>
+    <t>Mcallister, R C;Stimson, Blinnie;Mcallister, R</t>
   </si>
   <si>
     <t>Pavonia multiflora</t>
@@ -83,7 +83,7 @@
     <t>Takemoto, Roxie N</t>
   </si>
   <si>
-    <t>Fayre O'rourke;Madelle G Atkins;M Tanaka;M Lundberg;Nancee I Wolfman</t>
+    <t>O, Fayre;Atkins, Madelle G;Tanaka, M;Lundberg, M;Wolfman, Nancee I</t>
   </si>
   <si>
     <t>Agaricia fragilis;Lygodium japonicum;Sium suave</t>
@@ -107,7 +107,7 @@
     <t>Fitzgibbon, Ginelle M</t>
   </si>
   <si>
-    <t>Alvaro, Idalia C;Rochelle Caz Mcallister;Feany, C</t>
+    <t>Alvaro, Idalia C;Feany, C;Mcallister, Rochelle Caz</t>
   </si>
   <si>
     <t>Hasora vitta;Micrurus pyrrhocryptus</t>
@@ -119,7 +119,7 @@
     <t>Ninnetta J Teeven</t>
   </si>
   <si>
-    <t>Barrowman, Mallorie A;M Barrowman;Julietta A Lucretius;Irma Yankee Gay;Pugnaire, Shanta</t>
+    <t>Barrowman, Mallorie A;Pugnaire, Shanta;Barrowman, M;Lucretius, Julietta A;Gay, Irma Yankee</t>
   </si>
   <si>
     <t>Arctium lappa;Papio cynocephalus</t>
@@ -131,7 +131,7 @@
     <t>Reinagle, Nessi</t>
   </si>
   <si>
-    <t>Rochelle Caz Mcallister;Katerina Melack</t>
+    <t>Mcallister, Rochelle Caz;Melack, Katerina</t>
   </si>
   <si>
     <t>E. nevadensis;Lathyrus palustris;Amazilia cyanocephala</t>
@@ -143,7 +143,7 @@
     <t>Cabot, Eolanda</t>
   </si>
   <si>
-    <t>Marne Lundberg;Fayre Luce O'rourke</t>
+    <t>Lundberg, Marne;O, Fayre Luce</t>
   </si>
   <si>
     <t>Rosa chinensis</t>
@@ -155,7 +155,7 @@
     <t>Brecher, B</t>
   </si>
   <si>
-    <t>Shanta Dru Pugnaire;Caron Q Feany;Barrowman, Mallorie A;Lundberg, M G</t>
+    <t>Barrowman, Mallorie A;Lundberg, M G;Pugnaire, Shanta Dru;Feany, Caron Q</t>
   </si>
   <si>
     <t>Melitara prodenialis</t>
@@ -167,7 +167,7 @@
     <t>Teeven, Ninnetta J</t>
   </si>
   <si>
-    <t>Melisent D Mercola;Rochelle Caz Mcallister;Marne Giacopo Lundberg;Caron Feany;Rochelle Mcallister</t>
+    <t>Mercola, Melisent D;Mcallister, Rochelle Caz;Lundberg, Marne Giacopo;Feany, Caron;Mcallister, Rochelle</t>
   </si>
   <si>
     <t>Erythrophyllum delesserioides;Mortierella isabellina</t>
@@ -179,7 +179,7 @@
     <t>Pinero, Caril</t>
   </si>
   <si>
-    <t>M Atkins;Nancee Ingrim Wolfman;Barrowman, Mallorie</t>
+    <t>Barrowman, Mallorie;Atkins, M;Wolfman, Nancee Ingrim</t>
   </si>
   <si>
     <t>Bothrops pirajai;Ochotona thibetana</t>
@@ -191,7 +191,7 @@
     <t>Merralee Mcfarland</t>
   </si>
   <si>
-    <t>O'rourke, Fayre;O'rourke, Fayre L;Glimcher, Tomi;Lundberg, M;B Stimson</t>
+    <t>rourke, Fayre;rourke, Fayre L;Glimcher, Tomi;Lundberg, M;Stimson, B</t>
   </si>
   <si>
     <t>Trypanosoma vivax</t>
@@ -203,7 +203,7 @@
     <t>A Agresti</t>
   </si>
   <si>
-    <t>Shanta Dru Pugnaire</t>
+    <t>Pugnaire, Shanta Dru</t>
   </si>
   <si>
     <t>Salmonella berta;Xenocypris davidi;Diaeretiella rapae</t>
@@ -215,7 +215,7 @@
     <t>Hoppin, Sadye</t>
   </si>
   <si>
-    <t>Lundberg, M G;O'rourke, F L</t>
+    <t>Lundberg, M G;rourke, F L</t>
   </si>
   <si>
     <t>Cyamus boopis;Toxostoma redivivum;V. jobiensis</t>
@@ -227,7 +227,7 @@
     <t>Takemoto, Roxie</t>
   </si>
   <si>
-    <t>Feany, Caron;Gay, Irma;Chiquita J Wathelet</t>
+    <t>Feany, Caron;Gay, Irma;Wathelet, Chiquita J</t>
   </si>
   <si>
     <t>Erimacrus isenbeckii;P. hookeri;Telescopium telescopium</t>
@@ -239,7 +239,7 @@
     <t>Marsh, A</t>
   </si>
   <si>
-    <t>Idalia C Alvaro;Julietta A Lucretius;Julietta Alvy Lucretius;Penny Marius;Pugnaire, S D</t>
+    <t>Pugnaire, S D;Alvaro, Idalia C;Lucretius, Julietta A;Lucretius, Julietta Alvy;Marius, Penny</t>
   </si>
   <si>
     <t>Eucryptorrhynchus brandti;Murexechinus melanurus;Reishia clavigera</t>
@@ -251,7 +251,7 @@
     <t>Alicia H Uyterhoeven</t>
   </si>
   <si>
-    <t>Atkins, M G;Julietta A Lucretius;Caron Q Feany</t>
+    <t>Atkins, M G;Lucretius, Julietta A;Feany, Caron Q</t>
   </si>
   <si>
     <t>Sceloporus occidentalis</t>
@@ -275,7 +275,7 @@
     <t>Reinagle, N</t>
   </si>
   <si>
-    <t>Gay, I Y;Barrowman, M;Gay, Irma;Katerina Melack;Tanaka, M E</t>
+    <t>Gay, I Y;Barrowman, M;Gay, Irma;Tanaka, M E;Melack, Katerina</t>
   </si>
   <si>
     <t>Argas reflexus;Salmonella diarizonae</t>
@@ -287,7 +287,7 @@
     <t>Ashly Gav Saar</t>
   </si>
   <si>
-    <t>Penny E Marius</t>
+    <t>Marius, Penny E</t>
   </si>
   <si>
     <t>Bergeriella denitrificans;Tinamus guttatus;Ustilago sphaerogena</t>
@@ -296,7 +296,7 @@
     <t>Padgett, Nerita</t>
   </si>
   <si>
-    <t>Marne Giacopo Lundberg</t>
+    <t>Lundberg, Marne Giacopo</t>
   </si>
   <si>
     <t>Pyganodon grandis;Streptomyces kanamyceticus;Weissella hellenica</t>
@@ -308,7 +308,7 @@
     <t>Merralee I Mcfarland</t>
   </si>
   <si>
-    <t>Wolfman, N I;Rochelle C Mcallister;Alvaro, Idalia C;Gay, Irma Y</t>
+    <t>Wolfman, N I;Alvaro, Idalia C;Gay, Irma Y;Mcallister, Rochelle C</t>
   </si>
   <si>
     <t>Viola diffusa</t>
@@ -320,7 +320,7 @@
     <t>Breena Tulley Fogerty</t>
   </si>
   <si>
-    <t>I Alvaro;Musto, K;Marcella Ed Tanaka</t>
+    <t>Musto, K;Alvaro, I;Tanaka, Marcella Ed</t>
   </si>
   <si>
     <t>Furcifer minor;Lablab purpureus;Paracanthurus hepatus</t>
@@ -329,7 +329,7 @@
     <t>Starr, Tanhya</t>
   </si>
   <si>
-    <t>O'rourke, Fayre;Tomi D Glimcher;Atkins, Madelle;J Lucretius;C Feany</t>
+    <t>rourke, Fayre;Atkins, Madelle;Glimcher, Tomi D;Lucretius, J;Feany, C</t>
   </si>
   <si>
     <t>Leuconostoc mesenteroides;Gowidon temporalis</t>
@@ -353,7 +353,7 @@
     <t>Finnerty, M R</t>
   </si>
   <si>
-    <t>M Barrowman</t>
+    <t>Barrowman, M</t>
   </si>
   <si>
     <t>Conus villepinii;Haemophilus parasuis;Rhodopseudomonas palustris</t>
@@ -377,7 +377,7 @@
     <t>Tallie Schiada</t>
   </si>
   <si>
-    <t>Katharine E Musto;Alvaro, I C;Mercola, Melisent;Marne Lundberg</t>
+    <t>Alvaro, I C;Mercola, Melisent;Musto, Katharine E;Lundberg, Marne</t>
   </si>
   <si>
     <t>Euscaphis japonica;F. asiaticum</t>
@@ -389,7 +389,7 @@
     <t>Makepeace, N G</t>
   </si>
   <si>
-    <t>Marne Lundberg;Atkins, M G;Alvaro, I C;Fayre O'rourke;Mercola, Melisent D</t>
+    <t>Atkins, M G;Alvaro, I C;Mercola, Melisent D;Lundberg, Marne;O, Fayre</t>
   </si>
   <si>
     <t>Bornetella sphaerica;Crossoptilon crossoptilon</t>
@@ -413,7 +413,7 @@
     <t>Narayan, R</t>
   </si>
   <si>
-    <t>Tomi Damian Glimcher</t>
+    <t>Glimcher, Tomi Damian</t>
   </si>
   <si>
     <t>Tarsipes rostratus;Trinomys albispinus</t>
@@ -425,7 +425,7 @@
     <t>Rosalie G Narayan</t>
   </si>
   <si>
-    <t>Melack, Katerina;Mcallister, Rochelle;Feany, Caron;O'rourke, Fayre L</t>
+    <t>Melack, Katerina;Mcallister, Rochelle;Feany, Caron;rourke, Fayre L</t>
   </si>
   <si>
     <t>Dendropsophus ebraccatus;Gasterosteus aculeatus</t>
@@ -437,7 +437,7 @@
     <t>Westling, O</t>
   </si>
   <si>
-    <t>Wathelet, Chiquita J;Nancee I Wolfman;Melisent D Mercola;Melisent Mercola</t>
+    <t>Wathelet, Chiquita J;Wolfman, Nancee I;Mercola, Melisent D;Mercola, Melisent</t>
   </si>
   <si>
     <t>Anax junius;Drosophila narragansett;Lepidostoma togatum</t>
@@ -449,7 +449,7 @@
     <t>Waddington, K M</t>
   </si>
   <si>
-    <t>Wathelet, Chiquita;Shanta Dru Pugnaire;Musto, Katharine;Wathelet, Chiquita</t>
+    <t>Wathelet, Chiquita;Musto, Katharine;Wathelet, Chiquita;Pugnaire, Shanta Dru</t>
   </si>
   <si>
     <t>Callithrix geoffroyi;Ipomoea batatas;Phylloscopus fuscatus</t>
@@ -461,7 +461,7 @@
     <t>Waggener, Jessamyn</t>
   </si>
   <si>
-    <t>Glimcher, Tomi D;Irma Yankee Gay;R Mcallister;Idalia C Alvaro;Wathelet, C</t>
+    <t>Glimcher, Tomi D;Wathelet, C;Gay, Irma Yankee;Mcallister, R;Alvaro, Idalia C</t>
   </si>
   <si>
     <t>Athrotaxis laxifolia;Crossosoma bigelovii;Thrasops jacksonii</t>
@@ -473,7 +473,7 @@
     <t>Roskowick, Sidoney</t>
   </si>
   <si>
-    <t>Barrowman, Mallorie A;Alvaro, Idalia;Tomi Damian Glimcher;Alvaro, Idalia C;Julietta A Lucretius</t>
+    <t>Barrowman, Mallorie A;Alvaro, Idalia;Alvaro, Idalia C;Glimcher, Tomi Damian;Lucretius, Julietta A</t>
   </si>
   <si>
     <t>Dimorphotheca sinuata;Triaenodon obesus</t>
@@ -485,7 +485,7 @@
     <t>Malinde Kuliopulos</t>
   </si>
   <si>
-    <t>Barrowman, Mallorie;O'rourke, Fayre L;Stimson, B H;Gay, I Y</t>
+    <t>Barrowman, Mallorie;rourke, Fayre L;Stimson, B H;Gay, I Y</t>
   </si>
   <si>
     <t>H. ardens</t>
@@ -497,7 +497,7 @@
     <t>Marti Filip Perone</t>
   </si>
   <si>
-    <t>Idalia Alvaro</t>
+    <t>Alvaro, Idalia</t>
   </si>
   <si>
     <t>Fagus sylvatica</t>
@@ -509,7 +509,7 @@
     <t>C Pinero</t>
   </si>
   <si>
-    <t>Nancee Ingrim Wolfman;Lucretius, J;Barrowman, M A;Irma Y Gay</t>
+    <t>Lucretius, J;Barrowman, M A;Wolfman, Nancee Ingrim;Gay, Irma Y</t>
   </si>
   <si>
     <t>E. californica</t>
@@ -521,7 +521,7 @@
     <t>Kally M Waddington</t>
   </si>
   <si>
-    <t>Shanta Pugnaire</t>
+    <t>Pugnaire, Shanta</t>
   </si>
   <si>
     <t>Curculio hilgendorfi;Plasmodium knowlesi;Staphylea pinnata</t>
@@ -533,7 +533,7 @@
     <t>Sadye Hoppin</t>
   </si>
   <si>
-    <t>Melack, K;Lucretius, J A;Idalia Cirilo Alvaro;Gay, Irma Y</t>
+    <t>Melack, K;Lucretius, J A;Gay, Irma Y;Alvaro, Idalia Cirilo</t>
   </si>
   <si>
     <t>Arge nigripes;Physostegia virginiana;Platanthera ciliaris</t>
@@ -542,7 +542,7 @@
     <t>Hume, Tera</t>
   </si>
   <si>
-    <t>Chiquita Wathelet</t>
+    <t>Wathelet, Chiquita</t>
   </si>
   <si>
     <t>Diporiphora amphiboluroides;Pollachius virens;Kassina maculata</t>
@@ -554,9 +554,6 @@
     <t>E Cabot</t>
   </si>
   <si>
-    <t>Wathelet, Chiquita</t>
-  </si>
-  <si>
     <t>Abacion magnum;Paracanthurus hepatus</t>
   </si>
   <si>
@@ -566,7 +563,7 @@
     <t>Fara Fowler Trujillo</t>
   </si>
   <si>
-    <t>Melisent Derick Mercola;Gay, I</t>
+    <t>Gay, I;Mercola, Melisent Derick</t>
   </si>
   <si>
     <t>Dothistroma septosporum;Parantechinus apicalis</t>
@@ -578,7 +575,7 @@
     <t>Saar, Ashly</t>
   </si>
   <si>
-    <t>Mcallister, R C;Caron Q Feany;Tomi D Glimcher;Barrowman, M A;Pugnaire, Shanta D</t>
+    <t>Mcallister, R C;Barrowman, M A;Pugnaire, Shanta D;Feany, Caron Q;Glimcher, Tomi D</t>
   </si>
   <si>
     <t>Anolis distichus;Carabus glabratus;Macrobrachium olfersii</t>
@@ -590,7 +587,7 @@
     <t>Fogerty, Breena</t>
   </si>
   <si>
-    <t>Drake, Samantha;Barrowman, Mallorie;Gay, I;M Barrowman;Stimson, B</t>
+    <t>Drake, Samantha;Barrowman, Mallorie;Gay, I;Stimson, B;Barrowman, M</t>
   </si>
   <si>
     <t>Carcharhinus perezii;Maireana sedifolia</t>
@@ -611,7 +608,7 @@
     <t>Eolanda Pascal Cabot</t>
   </si>
   <si>
-    <t>Julietta Alvy Lucretius;Musto, K E;Irma Gay;Glimcher, T D;Mcallister, Rochelle C</t>
+    <t>Musto, K E;Glimcher, T D;Mcallister, Rochelle C;Lucretius, Julietta Alvy;Gay, Irma</t>
   </si>
   <si>
     <t>Chiroderma improvisum;Litoria fallax</t>
@@ -632,7 +629,7 @@
     <t>Falorsi, Kissiah</t>
   </si>
   <si>
-    <t>Katerina Weider Melack;Marius, P E</t>
+    <t>Marius, P E;Melack, Katerina Weider</t>
   </si>
   <si>
     <t>Peucaea mystacalis</t>
@@ -644,7 +641,7 @@
     <t>Kuliopulos, M</t>
   </si>
   <si>
-    <t>Marcella E Tanaka;Penny Elmer Marius;Rochelle Mcallister</t>
+    <t>Tanaka, Marcella E;Marius, Penny Elmer;Mcallister, Rochelle</t>
   </si>
   <si>
     <t>Otacanthus azureus;Pyrococcus endeavori;Trichomonas vaginalis</t>
@@ -668,7 +665,7 @@
     <t>Mel O Brenton</t>
   </si>
   <si>
-    <t>Marcella Ed Tanaka;Gay, Irma</t>
+    <t>Gay, Irma;Tanaka, Marcella Ed</t>
   </si>
   <si>
     <t>Calopteryx virgo</t>
@@ -680,7 +677,7 @@
     <t>Franny C Stephanos</t>
   </si>
   <si>
-    <t>Mercola, M;Pugnaire, Shanta D;Katerina Melack;Julietta A Lucretius;Irma Yankee Gay</t>
+    <t>Mercola, M;Pugnaire, Shanta D;Melack, Katerina;Lucretius, Julietta A;Gay, Irma Yankee</t>
   </si>
   <si>
     <t>Debregeasia longifolia</t>
@@ -692,7 +689,7 @@
     <t>Mcfarland, Merralee</t>
   </si>
   <si>
-    <t>Mercola, Melisent D;Melack, Katerina W;Drake, S;T Glimcher</t>
+    <t>Mercola, Melisent D;Melack, Katerina W;Drake, S;Glimcher, T</t>
   </si>
   <si>
     <t>Canthigaster valentini;Rhopalomyia pomum;Stachybotrys chartarum</t>
@@ -704,7 +701,7 @@
     <t>Christian E Keller</t>
   </si>
   <si>
-    <t>Mallorie Barrowman;Drake, S D;C Wathelet;Melack, K W</t>
+    <t>Drake, S D;Melack, K W;Barrowman, Mallorie;Wathelet, C</t>
   </si>
   <si>
     <t>Fluoribacter bozemanae;Kocuria rosea</t>
@@ -716,7 +713,7 @@
     <t>Merola Finnerty</t>
   </si>
   <si>
-    <t>J Lucretius;Marius, P;Katharine E Musto;Chiquita Wathelet;Drake, Samantha D</t>
+    <t>Marius, P;Drake, Samantha D;Lucretius, J;Musto, Katharine E;Wathelet, Chiquita</t>
   </si>
   <si>
     <t>Guarianthe aurantiaca</t>
@@ -728,7 +725,7 @@
     <t>Cabot, Eolanda P</t>
   </si>
   <si>
-    <t>O'rourke, F;Julietta Alvy Lucretius</t>
+    <t>rourke, F;Lucretius, Julietta Alvy</t>
   </si>
   <si>
     <t>Podarcis siculus;Rhyzopertha dominica</t>
@@ -740,7 +737,7 @@
     <t>Takemoto, R</t>
   </si>
   <si>
-    <t>Barrowman, M;M Lundberg;Drake, S;I Alvaro;M Lundberg</t>
+    <t>Barrowman, M;Drake, S;Lundberg, M;Alvaro, I;Lundberg, M</t>
   </si>
   <si>
     <t>Oniscus asellus;Pandalopsis japonica</t>
@@ -764,7 +761,7 @@
     <t>Fogerty, B T</t>
   </si>
   <si>
-    <t>M Lundberg;M Barrowman;Glimcher, Tomi;Chiquita Joel Wathelet;Caron Q Feany</t>
+    <t>Glimcher, Tomi;Lundberg, M;Barrowman, M;Wathelet, Chiquita Joel;Feany, Caron Q</t>
   </si>
   <si>
     <t>Anopheles freeborni;Bassiana duperreyi</t>
@@ -776,7 +773,7 @@
     <t>Fara F Trujillo</t>
   </si>
   <si>
-    <t>O'rourke, F;Feany, C Q</t>
+    <t>rourke, F;Feany, C Q</t>
   </si>
   <si>
     <t>Lavandula lanata</t>
@@ -788,7 +785,7 @@
     <t>Rosalie Narayan</t>
   </si>
   <si>
-    <t>Madelle Atkins;Feany, Caron;S Drake;Irma Y Gay</t>
+    <t>Feany, Caron;Atkins, Madelle;Drake, S;Gay, Irma Y</t>
   </si>
   <si>
     <t>Ephippiorhynchus asiaticus</t>
@@ -806,7 +803,7 @@
     <t>Remillard, Iona</t>
   </si>
   <si>
-    <t>Caron Q Feany</t>
+    <t>Feany, Caron Q</t>
   </si>
   <si>
     <t>Lathyrus tingitanus;Ophryotrocha labronica</t>
@@ -818,7 +815,7 @@
     <t>Brenton, M O</t>
   </si>
   <si>
-    <t>C Feany;Marcella Tanaka;Nancee Wolfman;Wolfman, Nancee</t>
+    <t>Wolfman, Nancee;Feany, C;Tanaka, Marcella;Wolfman, Nancee</t>
   </si>
   <si>
     <t>Calyptophilus frugivorus;Chrysopa lezeyi;Otus gurneyi</t>
@@ -830,7 +827,7 @@
     <t>Hoppin, S M</t>
   </si>
   <si>
-    <t>Glimcher, Tomi D;Nancee I Wolfman;Feany, Caron;Katharine Erskine Musto;Atkins, M G</t>
+    <t>Glimcher, Tomi D;Feany, Caron;Atkins, M G;Wolfman, Nancee I;Musto, Katharine Erskine</t>
   </si>
   <si>
     <t>Centropyge potteri;Chrysogaster solstitialis;Hyalophora euryalus</t>
@@ -842,7 +839,7 @@
     <t>Nessi Delmar Reinagle</t>
   </si>
   <si>
-    <t>Rochelle Mcallister;Lundberg, Marne;S Pugnaire</t>
+    <t>Lundberg, Marne;Mcallister, Rochelle;Pugnaire, S</t>
   </si>
   <si>
     <t>M. neglecta;P. peregrinus</t>
@@ -866,7 +863,7 @@
     <t>Agresti, Alfy</t>
   </si>
   <si>
-    <t>Chiquita Joel Wathelet;Melisent D Mercola;Julietta Alvy Lucretius</t>
+    <t>Wathelet, Chiquita Joel;Mercola, Melisent D;Lucretius, Julietta Alvy</t>
   </si>
   <si>
     <t>Mesopodopsis slabberi</t>
@@ -875,7 +872,7 @@
     <t>Gauthier, Delphine</t>
   </si>
   <si>
-    <t>Drake, S D;Penny E Marius;Chiquita Wathelet</t>
+    <t>Drake, S D;Marius, Penny E;Wathelet, Chiquita</t>
   </si>
   <si>
     <t>Apus apus;Mucuna pruriens;R. pulchra</t>
@@ -887,7 +884,7 @@
     <t>B Fogerty</t>
   </si>
   <si>
-    <t>Mallorie Barrowman;Marius, P E</t>
+    <t>Marius, P E;Barrowman, Mallorie</t>
   </si>
   <si>
     <t>Cephalophus rubidus;H. lunaris;Tetrahymena australis</t>
@@ -896,7 +893,7 @@
     <t>Polverini, Clara</t>
   </si>
   <si>
-    <t>Gay, Irma;Melack, K;Samantha D Drake</t>
+    <t>Gay, Irma;Melack, K;Drake, Samantha D</t>
   </si>
   <si>
     <t>P. adspersus</t>
@@ -908,7 +905,7 @@
     <t>Berget Brecher</t>
   </si>
   <si>
-    <t>Feany, Caron Q;Wathelet, Chiquita;Penny E Marius;Katerina Weider Melack</t>
+    <t>Feany, Caron Q;Wathelet, Chiquita;Marius, Penny E;Melack, Katerina Weider</t>
   </si>
   <si>
     <t>Ctenomys goodfellowi;Pleuronichthys cornutus;Plexaura homomalla</t>
@@ -920,7 +917,7 @@
     <t>S Dame</t>
   </si>
   <si>
-    <t>Katerina Melack;M Tanaka</t>
+    <t>Melack, Katerina;Tanaka, M</t>
   </si>
   <si>
     <t>Thelephora ganbajun</t>
@@ -932,7 +929,7 @@
     <t>Kuliopulos, Malinde T</t>
   </si>
   <si>
-    <t>M Tanaka</t>
+    <t>Tanaka, M</t>
   </si>
   <si>
     <t>Eucalyptus microcorys;Pyura stolonifera</t>
@@ -941,7 +938,7 @@
     <t>Kreisberg, Lucina</t>
   </si>
   <si>
-    <t>Katerina Melack</t>
+    <t>Melack, Katerina</t>
   </si>
   <si>
     <t>Devario pathirana;Eulemur coronatus</t>
@@ -953,7 +950,7 @@
     <t>Kuliopulos, M T</t>
   </si>
   <si>
-    <t>Mcallister, R;Melisent Mercola</t>
+    <t>Mcallister, R;Mercola, Melisent</t>
   </si>
   <si>
     <t>Cystopteris fragilis;Torgos tracheliotos</t>
@@ -965,7 +962,7 @@
     <t>F Stephanos</t>
   </si>
   <si>
-    <t>Musto, Katharine;Caron Quentin Feany;Shanta D Pugnaire;Irma Yankee Gay;Penny Elmer Marius</t>
+    <t>Musto, Katharine;Feany, Caron Quentin;Pugnaire, Shanta D;Gay, Irma Yankee;Marius, Penny Elmer</t>
   </si>
   <si>
     <t>Agathis moorei;Keckiella cordifolia;Trachylepis maculilabris</t>
@@ -977,7 +974,7 @@
     <t>Narayan, Rosalie G</t>
   </si>
   <si>
-    <t>Lucretius, J;Pugnaire, Shanta D;Blinnie Stimson;Barrowman, M;Wolfman, N I</t>
+    <t>Lucretius, J;Pugnaire, Shanta D;Barrowman, M;Wolfman, N I;Stimson, Blinnie</t>
   </si>
   <si>
     <t>B. vulgaris;Rickettsia slovaca</t>
@@ -995,7 +992,7 @@
     <t>Plasket, Verina</t>
   </si>
   <si>
-    <t>Chiquita Wathelet;Musto, Katharine</t>
+    <t>Musto, Katharine;Wathelet, Chiquita</t>
   </si>
   <si>
     <t>Nepenthes distillatoria</t>
@@ -1007,7 +1004,7 @@
     <t>Perone, Marti</t>
   </si>
   <si>
-    <t>Feany, C Q;I Gay;F O'rourke;Shanta D Pugnaire;Julietta Lucretius</t>
+    <t>Feany, C Q;Gay, I;O, F;Pugnaire, Shanta D;Lucretius, Julietta</t>
   </si>
   <si>
     <t>Botrylloides violaceus;Furcifer balteatus;Petaurista albiventer</t>
@@ -1016,7 +1013,7 @@
     <t>Vishik, Terese</t>
   </si>
   <si>
-    <t>C Wathelet</t>
+    <t>Wathelet, C</t>
   </si>
   <si>
     <t>Egretta novaehollandiae;Mentha australis;Rotylenchulus reniformis</t>
@@ -1028,7 +1025,7 @@
     <t>Sue Dame</t>
   </si>
   <si>
-    <t>Wolfman, Nancee;Nancee I Wolfman</t>
+    <t>Wolfman, Nancee;Wolfman, Nancee I</t>
   </si>
   <si>
     <t>Molva molva</t>
@@ -1049,7 +1046,7 @@
     <t>O Westling</t>
   </si>
   <si>
-    <t>Fayre O'rourke</t>
+    <t>O, Fayre</t>
   </si>
   <si>
     <t>Anigozanthos flavidus;Chelonibia testudinaria</t>
@@ -1061,7 +1058,7 @@
     <t>Fara Trujillo</t>
   </si>
   <si>
-    <t>P Marius;Lucretius, J</t>
+    <t>Lucretius, J;Marius, P</t>
   </si>
   <si>
     <t>Bodianus oxycephalus;Corvus corax</t>
@@ -1070,7 +1067,7 @@
     <t>Gerardi, Adele</t>
   </si>
   <si>
-    <t>Mercola, Melisent D;Shanta Pugnaire;M Tanaka;Atkins, Madelle;C Wathelet</t>
+    <t>Mercola, Melisent D;Atkins, Madelle;Pugnaire, Shanta;Tanaka, M;Wathelet, C</t>
   </si>
   <si>
     <t>Mycobacterium shimoidei</t>
@@ -1091,7 +1088,7 @@
     <t>Marti Perone</t>
   </si>
   <si>
-    <t>Wathelet, C J;Samantha Demetre Drake;Penny Elmer Marius;Feany, Caron</t>
+    <t>Wathelet, C J;Feany, Caron;Drake, Samantha Demetre;Marius, Penny Elmer</t>
   </si>
   <si>
     <t>Adesmia lanata</t>
@@ -1100,7 +1097,7 @@
     <t>Manser, Quinta</t>
   </si>
   <si>
-    <t>Musto, K E;T Glimcher;Julietta Lucretius;Gay, I Y</t>
+    <t>Musto, K E;Gay, I Y;Glimcher, T;Lucretius, Julietta</t>
   </si>
   <si>
     <t>Anopheles merus;Bodo saltans</t>
@@ -1112,7 +1109,7 @@
     <t>S Roskowick</t>
   </si>
   <si>
-    <t>Nancee Wolfman</t>
+    <t>Wolfman, Nancee</t>
   </si>
   <si>
     <t>Chamaecrista fasciculata;Streptococcus intermedius</t>
@@ -1124,7 +1121,7 @@
     <t>Sidoney J Roskowick</t>
   </si>
   <si>
-    <t>Mercola, M;T Glimcher;Mcallister, R;Tanaka, M</t>
+    <t>Mercola, M;Mcallister, R;Tanaka, M;Glimcher, T</t>
   </si>
   <si>
     <t>Chaerephon nigeriae</t>
@@ -1136,7 +1133,7 @@
     <t>Agresti, A A</t>
   </si>
   <si>
-    <t>Katharine Erskine Musto;Glimcher, Tomi D;Caron Q Feany</t>
+    <t>Glimcher, Tomi D;Musto, Katharine Erskine;Feany, Caron Q</t>
   </si>
   <si>
     <t>Pipistrellus pygmaeus</t>
@@ -1145,7 +1142,7 @@
     <t>Guida, Julianne</t>
   </si>
   <si>
-    <t>Mallorie A Barrowman</t>
+    <t>Barrowman, Mallorie A</t>
   </si>
   <si>
     <t>Datana perspicua</t>
@@ -1157,7 +1154,7 @@
     <t>Christian Ellsworth Keller</t>
   </si>
   <si>
-    <t>M Lundberg;Caron Quentin Feany;Melack, K W;Melisent D Mercola;Lundberg, M</t>
+    <t>Melack, K W;Lundberg, M;Lundberg, M;Feany, Caron Quentin;Mercola, Melisent D</t>
   </si>
   <si>
     <t>S. magellanicus</t>
@@ -2302,10 +2299,10 @@
         <v>178</v>
       </c>
       <c r="D46" t="s">
+        <v>175</v>
+      </c>
+      <c r="E46" t="s">
         <v>179</v>
-      </c>
-      <c r="E46" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2313,16 +2310,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" t="s">
         <v>181</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>182</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>183</v>
-      </c>
-      <c r="E47" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2330,16 +2327,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" t="s">
         <v>185</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>186</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>187</v>
-      </c>
-      <c r="E48" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2347,16 +2344,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" t="s">
         <v>189</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>190</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>191</v>
-      </c>
-      <c r="E49" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2364,16 +2361,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" t="s">
         <v>193</v>
-      </c>
-      <c r="C50" t="s">
-        <v>194</v>
       </c>
       <c r="D50" t="s">
         <v>116</v>
       </c>
       <c r="E50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2381,16 +2378,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" t="s">
         <v>196</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>197</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>198</v>
-      </c>
-      <c r="E51" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2398,16 +2395,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" t="s">
         <v>200</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>201</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>202</v>
-      </c>
-      <c r="E52" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2415,16 +2412,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C53" t="s">
         <v>111</v>
       </c>
       <c r="D53" t="s">
+        <v>204</v>
+      </c>
+      <c r="E53" t="s">
         <v>205</v>
-      </c>
-      <c r="E53" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2432,16 +2429,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" t="s">
         <v>207</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>208</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>209</v>
-      </c>
-      <c r="E54" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2449,16 +2446,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
+        <v>210</v>
+      </c>
+      <c r="C55" t="s">
         <v>211</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>212</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>213</v>
-      </c>
-      <c r="E55" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2466,16 +2463,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" t="s">
         <v>215</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>216</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>217</v>
-      </c>
-      <c r="E56" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2483,16 +2480,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
+        <v>218</v>
+      </c>
+      <c r="C57" t="s">
         <v>219</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>220</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>221</v>
-      </c>
-      <c r="E57" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2500,16 +2497,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
+        <v>222</v>
+      </c>
+      <c r="C58" t="s">
         <v>223</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>224</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>225</v>
-      </c>
-      <c r="E58" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2517,16 +2514,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
+        <v>226</v>
+      </c>
+      <c r="C59" t="s">
         <v>227</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>228</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>229</v>
-      </c>
-      <c r="E59" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2534,16 +2531,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
+        <v>230</v>
+      </c>
+      <c r="C60" t="s">
         <v>231</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>232</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>233</v>
-      </c>
-      <c r="E60" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2551,16 +2548,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
+        <v>234</v>
+      </c>
+      <c r="C61" t="s">
         <v>235</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>236</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>237</v>
-      </c>
-      <c r="E61" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2568,16 +2565,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
+        <v>238</v>
+      </c>
+      <c r="C62" t="s">
         <v>239</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>240</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>241</v>
-      </c>
-      <c r="E62" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2585,16 +2582,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
+        <v>242</v>
+      </c>
+      <c r="C63" t="s">
         <v>243</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>244</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>245</v>
-      </c>
-      <c r="E63" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2602,16 +2599,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>246</v>
+      </c>
+      <c r="C64" t="s">
         <v>247</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>248</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>249</v>
-      </c>
-      <c r="E64" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2619,16 +2616,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>250</v>
+      </c>
+      <c r="C65" t="s">
         <v>251</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>252</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>253</v>
-      </c>
-      <c r="E65" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2636,16 +2633,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>254</v>
+      </c>
+      <c r="C66" t="s">
         <v>255</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>256</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>257</v>
-      </c>
-      <c r="E66" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2653,16 +2650,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>258</v>
+      </c>
+      <c r="C67" t="s">
         <v>259</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
+        <v>175</v>
+      </c>
+      <c r="E67" t="s">
         <v>260</v>
-      </c>
-      <c r="D67" t="s">
-        <v>179</v>
-      </c>
-      <c r="E67" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2670,16 +2667,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C68" t="s">
         <v>69</v>
       </c>
       <c r="D68" t="s">
+        <v>262</v>
+      </c>
+      <c r="E68" t="s">
         <v>263</v>
-      </c>
-      <c r="E68" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2687,16 +2684,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" t="s">
         <v>265</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>266</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>267</v>
-      </c>
-      <c r="E69" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2704,16 +2701,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>268</v>
+      </c>
+      <c r="C70" t="s">
         <v>269</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>270</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>271</v>
-      </c>
-      <c r="E70" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2721,16 +2718,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
+        <v>272</v>
+      </c>
+      <c r="C71" t="s">
         <v>273</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>274</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>275</v>
-      </c>
-      <c r="E71" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2738,16 +2735,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
+        <v>276</v>
+      </c>
+      <c r="C72" t="s">
         <v>277</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>278</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>279</v>
-      </c>
-      <c r="E72" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2755,16 +2752,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
+        <v>280</v>
+      </c>
+      <c r="C73" t="s">
         <v>281</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>282</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>283</v>
-      </c>
-      <c r="E73" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2772,16 +2769,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
+        <v>284</v>
+      </c>
+      <c r="C74" t="s">
+        <v>185</v>
+      </c>
+      <c r="D74" t="s">
         <v>285</v>
       </c>
-      <c r="C74" t="s">
-        <v>186</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>286</v>
-      </c>
-      <c r="E74" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2789,16 +2786,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
+        <v>287</v>
+      </c>
+      <c r="C75" t="s">
         <v>288</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>289</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>290</v>
-      </c>
-      <c r="E75" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2806,16 +2803,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C76" t="s">
         <v>100</v>
       </c>
       <c r="D76" t="s">
+        <v>292</v>
+      </c>
+      <c r="E76" t="s">
         <v>293</v>
-      </c>
-      <c r="E76" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2823,16 +2820,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
+        <v>294</v>
+      </c>
+      <c r="C77" t="s">
         <v>295</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>296</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>297</v>
-      </c>
-      <c r="E77" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2840,16 +2837,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
+        <v>298</v>
+      </c>
+      <c r="C78" t="s">
         <v>299</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>300</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>301</v>
-      </c>
-      <c r="E78" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2857,16 +2854,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
+        <v>302</v>
+      </c>
+      <c r="C79" t="s">
         <v>303</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>304</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>305</v>
-      </c>
-      <c r="E79" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2874,16 +2871,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C80" t="s">
         <v>163</v>
       </c>
       <c r="D80" t="s">
+        <v>307</v>
+      </c>
+      <c r="E80" t="s">
         <v>308</v>
-      </c>
-      <c r="E80" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2891,16 +2888,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
+        <v>309</v>
+      </c>
+      <c r="C81" t="s">
         <v>310</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>311</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>312</v>
-      </c>
-      <c r="E81" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2908,16 +2905,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
+        <v>313</v>
+      </c>
+      <c r="C82" t="s">
         <v>314</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>315</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>316</v>
-      </c>
-      <c r="E82" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2925,16 +2922,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
+        <v>317</v>
+      </c>
+      <c r="C83" t="s">
         <v>318</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>319</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>320</v>
-      </c>
-      <c r="E83" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2942,16 +2939,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C84" t="s">
         <v>21</v>
       </c>
       <c r="D84" t="s">
+        <v>322</v>
+      </c>
+      <c r="E84" t="s">
         <v>323</v>
-      </c>
-      <c r="E84" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2959,16 +2956,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
+        <v>324</v>
+      </c>
+      <c r="C85" t="s">
+        <v>281</v>
+      </c>
+      <c r="D85" t="s">
         <v>325</v>
       </c>
-      <c r="C85" t="s">
-        <v>282</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>326</v>
-      </c>
-      <c r="E85" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2976,16 +2973,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
+        <v>327</v>
+      </c>
+      <c r="C86" t="s">
         <v>328</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>329</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>330</v>
-      </c>
-      <c r="E86" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2993,16 +2990,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
+        <v>331</v>
+      </c>
+      <c r="C87" t="s">
+        <v>259</v>
+      </c>
+      <c r="D87" t="s">
         <v>332</v>
       </c>
-      <c r="C87" t="s">
-        <v>260</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>333</v>
-      </c>
-      <c r="E87" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3010,16 +3007,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
+        <v>334</v>
+      </c>
+      <c r="C88" t="s">
         <v>335</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>336</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>337</v>
-      </c>
-      <c r="E88" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -3027,16 +3024,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
+        <v>338</v>
+      </c>
+      <c r="C89" t="s">
         <v>339</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
+        <v>304</v>
+      </c>
+      <c r="E89" t="s">
         <v>340</v>
-      </c>
-      <c r="D89" t="s">
-        <v>305</v>
-      </c>
-      <c r="E89" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -3044,16 +3041,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
+        <v>341</v>
+      </c>
+      <c r="C90" t="s">
         <v>342</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>343</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>344</v>
-      </c>
-      <c r="E90" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -3061,16 +3058,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
+        <v>345</v>
+      </c>
+      <c r="C91" t="s">
         <v>346</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>347</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>348</v>
-      </c>
-      <c r="E91" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -3078,16 +3075,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C92" t="s">
         <v>171</v>
       </c>
       <c r="D92" t="s">
+        <v>350</v>
+      </c>
+      <c r="E92" t="s">
         <v>351</v>
-      </c>
-      <c r="E92" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -3095,16 +3092,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
+        <v>352</v>
+      </c>
+      <c r="C93" t="s">
         <v>353</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
+        <v>332</v>
+      </c>
+      <c r="E93" t="s">
         <v>354</v>
-      </c>
-      <c r="D93" t="s">
-        <v>333</v>
-      </c>
-      <c r="E93" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -3112,16 +3109,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
+        <v>355</v>
+      </c>
+      <c r="C94" t="s">
         <v>356</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>357</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>358</v>
-      </c>
-      <c r="E94" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -3129,16 +3126,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
+        <v>359</v>
+      </c>
+      <c r="C95" t="s">
+        <v>295</v>
+      </c>
+      <c r="D95" t="s">
         <v>360</v>
       </c>
-      <c r="C95" t="s">
-        <v>296</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>361</v>
-      </c>
-      <c r="E95" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -3146,16 +3143,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
+        <v>362</v>
+      </c>
+      <c r="C96" t="s">
         <v>363</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>364</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>365</v>
-      </c>
-      <c r="E96" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -3163,16 +3160,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
+        <v>366</v>
+      </c>
+      <c r="C97" t="s">
         <v>367</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>368</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>369</v>
-      </c>
-      <c r="E97" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -3180,16 +3177,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
+        <v>370</v>
+      </c>
+      <c r="C98" t="s">
         <v>371</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>372</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>373</v>
-      </c>
-      <c r="E98" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -3197,16 +3194,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C99" t="s">
         <v>159</v>
       </c>
       <c r="D99" t="s">
+        <v>375</v>
+      </c>
+      <c r="E99" t="s">
         <v>376</v>
-      </c>
-      <c r="E99" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -3214,16 +3211,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
+        <v>377</v>
+      </c>
+      <c r="C100" t="s">
         <v>378</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>379</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>380</v>
-      </c>
-      <c r="E100" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -3231,16 +3228,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
+        <v>381</v>
+      </c>
+      <c r="C101" t="s">
         <v>382</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>383</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>384</v>
-      </c>
-      <c r="E101" t="s">
-        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>